<commit_message>
Add all changes from the other repo
</commit_message>
<xml_diff>
--- a/raw_data/table_2.xlsx
+++ b/raw_data/table_2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="0" windowWidth="37470" windowHeight="18420"/>
+    <workbookView xWindow="3720" yWindow="0" windowWidth="37470" windowHeight="18420"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -1871,8 +1871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="Y9" sqref="Y9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Y13" sqref="Y13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>